<commit_message>
Font taken from excel
</commit_message>
<xml_diff>
--- a/GenreFontDataset.xlsx
+++ b/GenreFontDataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noemi\Documents\GitHub\LyriFont\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleferro98/PycharmProjects/pythonProject1/LyriFont/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23486DC7-F9BF-41B0-A9AD-FA4542931444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F234CCB9-F0BC-2F4E-A3B1-CF33DB6071FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A15F46D3-8475-C34D-B725-AC13240FCFA4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{A15F46D3-8475-C34D-B725-AC13240FCFA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
   <si>
     <t>Music Genre</t>
   </si>
@@ -367,6 +367,12 @@
   </si>
   <si>
     <t>Mighty-X34Z2.ttf</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Tempo</t>
   </si>
 </sst>
 </file>
@@ -448,9 +454,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -488,7 +494,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -594,7 +600,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -736,7 +742,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -744,27 +750,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC8A9F8-F6F7-C446-981F-A14B4FAC156C}">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="85.875" customWidth="1"/>
-    <col min="2" max="2" width="86.625" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -772,7 +785,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -780,7 +793,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -788,7 +801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -796,7 +809,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -804,7 +817,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -812,7 +825,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -820,7 +833,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -828,7 +841,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -836,7 +849,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -844,7 +857,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -852,7 +865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -860,7 +873,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -868,7 +881,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -876,7 +889,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -884,7 +897,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -892,7 +905,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -900,7 +913,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -908,7 +921,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -916,7 +929,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -924,7 +937,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -932,7 +945,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -940,7 +953,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -948,7 +961,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -956,7 +969,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -964,7 +977,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -972,7 +985,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -980,7 +993,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -988,7 +1001,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -996,7 +1009,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1004,7 +1017,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1012,7 +1025,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -1020,7 +1033,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1028,7 +1041,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1036,7 +1049,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1044,7 +1057,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1052,7 +1065,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1060,7 +1073,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1068,7 +1081,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1076,7 +1089,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1084,7 +1097,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1092,7 +1105,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1100,7 +1113,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1108,7 +1121,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -1116,7 +1129,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1124,7 +1137,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1132,7 +1145,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -1140,7 +1153,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -1148,7 +1161,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -1156,7 +1169,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -1164,7 +1177,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -1172,7 +1185,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -1180,7 +1193,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -1188,7 +1201,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -1196,7 +1209,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -1204,7 +1217,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -1212,7 +1225,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -1220,7 +1233,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -1228,7 +1241,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -1236,7 +1249,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -1244,7 +1257,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -1252,7 +1265,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -1260,7 +1273,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -1268,7 +1281,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -1276,7 +1289,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -1284,7 +1297,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -1292,7 +1305,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -1300,7 +1313,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -1308,7 +1321,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -1316,7 +1329,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>9</v>
       </c>
@@ -1324,7 +1337,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>9</v>
       </c>
@@ -1332,7 +1345,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>9</v>
       </c>
@@ -1340,7 +1353,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>9</v>
       </c>
@@ -1348,7 +1361,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>9</v>
       </c>
@@ -1356,7 +1369,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>9</v>
       </c>
@@ -1364,7 +1377,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>9</v>
       </c>
@@ -1372,7 +1385,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>9</v>
       </c>
@@ -1380,7 +1393,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>9</v>
       </c>
@@ -1388,7 +1401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>9</v>
       </c>
@@ -1396,7 +1409,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>10</v>
       </c>
@@ -1404,7 +1417,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>10</v>
       </c>
@@ -1412,7 +1425,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>10</v>
       </c>
@@ -1420,7 +1433,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -1428,7 +1441,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -1436,7 +1449,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>10</v>
       </c>
@@ -1444,7 +1457,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>10</v>
       </c>
@@ -1452,7 +1465,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>10</v>
       </c>
@@ -1460,7 +1473,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>10</v>
       </c>
@@ -1468,7 +1481,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>10</v>
       </c>
@@ -1476,7 +1489,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>11</v>
       </c>
@@ -1484,7 +1497,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>11</v>
       </c>
@@ -1492,7 +1505,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>11</v>
       </c>
@@ -1500,7 +1513,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>11</v>
       </c>
@@ -1508,7 +1521,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>11</v>
       </c>
@@ -1516,7 +1529,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>11</v>
       </c>
@@ -1524,7 +1537,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -1532,7 +1545,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>11</v>
       </c>
@@ -1540,7 +1553,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>11</v>
       </c>
@@ -1548,7 +1561,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
OTF to TTF extension changed
</commit_message>
<xml_diff>
--- a/GenreFontDataset.xlsx
+++ b/GenreFontDataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleferro98/PycharmProjects/pythonProject1/LyriFont/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleferro98/Desktop/LyriFont-May2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F234CCB9-F0BC-2F4E-A3B1-CF33DB6071FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D8448A-3AFB-A04E-A0F2-ECC4DCBE0FD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{A15F46D3-8475-C34D-B725-AC13240FCFA4}"/>
   </bookViews>
@@ -93,12 +93,6 @@
     <t>RockPlaza-517M8.ttf</t>
   </si>
   <si>
-    <t>RockRadio-Wy4Vz.otf</t>
-  </si>
-  <si>
-    <t>RockSlayers-BW6Lw.otf</t>
-  </si>
-  <si>
     <t>RockSteady-Wyy7A.ttf</t>
   </si>
   <si>
@@ -126,21 +120,12 @@
     <t>RoundPop-owwjd.ttf</t>
   </si>
   <si>
-    <t>TigerChest-yw6Le.otf</t>
-  </si>
-  <si>
     <t>UnicornPop-Z0qq.ttf</t>
   </si>
   <si>
     <t>BogartsMetal-MVBEe.ttf</t>
   </si>
   <si>
-    <t>CrushMetal-8MP7A.otf</t>
-  </si>
-  <si>
-    <t>DeadeldermetalRegular-1Gx3v.otf</t>
-  </si>
-  <si>
     <t>Distem-VG2nx.ttf</t>
   </si>
   <si>
@@ -168,21 +153,12 @@
     <t>AttackGraffiti-3zRBM.ttf</t>
   </si>
   <si>
-    <t>BombDaGone-VG0RB.otf</t>
-  </si>
-  <si>
     <t>Chronic-1GnwL.ttf</t>
   </si>
   <si>
-    <t>DonGraffiti-wrYx.otf</t>
-  </si>
-  <si>
     <t>DowntownStreet-0WY0R.ttf</t>
   </si>
   <si>
-    <t>GraffitiHipsterDemoVersionRegular-ZVBxJ.otf</t>
-  </si>
-  <si>
     <t>SlimWandalsAltPersonalUse-AL9vM.ttf</t>
   </si>
   <si>
@@ -222,42 +198,18 @@
     <t>SuperCool-MVg1p.ttf</t>
   </si>
   <si>
-    <t>AutumnFlowers-9YVZK.otf</t>
-  </si>
-  <si>
     <t>BabySela-vmxz4.ttf</t>
   </si>
   <si>
-    <t>ClassicSignatureDemo-axdDE.otf</t>
-  </si>
-  <si>
-    <t>Classical-4pq9.otf</t>
-  </si>
-  <si>
-    <t>ElegantDemo-OVJX6.otf</t>
-  </si>
-  <si>
-    <t>ElegantStylish-JR3xj.otf</t>
-  </si>
-  <si>
-    <t>Faldith-qZM95.otf</t>
-  </si>
-  <si>
     <t>FathirScriptPersonalUseOnly-MV2rJ.ttf</t>
   </si>
   <si>
     <t>HarmonyStrikinglyRegular-d978X.ttf</t>
   </si>
   <si>
-    <t>RusillaSerif-2OZpl.otf</t>
-  </si>
-  <si>
     <t>AguaDejamaicaItalic-55Yv.ttf</t>
   </si>
   <si>
-    <t>MarleyRegular-zM1a.otf</t>
-  </si>
-  <si>
     <t>MarleyFontDemoDemo-eZDVO.ttf</t>
   </si>
   <si>
@@ -270,15 +222,6 @@
     <t>TunUpDeTing-jBxy.ttf</t>
   </si>
   <si>
-    <t>70SdiscopersonaluseBold-w14z2.otf</t>
-  </si>
-  <si>
-    <t>DiscoDeck-a4wa.otf</t>
-  </si>
-  <si>
-    <t>DiscoDuck3DItalic-al1m.otf</t>
-  </si>
-  <si>
     <t>DiscoEverydayValueRegular-zMGG.ttf</t>
   </si>
   <si>
@@ -291,27 +234,15 @@
     <t>Gelam-lKo5.ttf</t>
   </si>
   <si>
-    <t>MoogieDisco-2OwAX.otf</t>
-  </si>
-  <si>
     <t>Sugar-lxD5.ttf</t>
   </si>
   <si>
     <t>TokyoHoneyChan-dLR.ttf</t>
   </si>
   <si>
-    <t>BeautySwingPersonalUse-DOEaD.otf</t>
-  </si>
-  <si>
     <t>jazztext.ttf</t>
   </si>
   <si>
-    <t>MEllington.otf</t>
-  </si>
-  <si>
-    <t>OPTINovelGothic-XBoldAgen.otf</t>
-  </si>
-  <si>
     <t>FieldsOfCathayRegular-Z9B3.ttf</t>
   </si>
   <si>
@@ -327,15 +258,9 @@
     <t>RoadShot-qZYDl.ttf</t>
   </si>
   <si>
-    <t>RumbleweedspurRegular-VwLy.otf</t>
-  </si>
-  <si>
     <t>TheCheelaved-owOvo.ttf</t>
   </si>
   <si>
-    <t>UnchainedRoughPersonalUseRegular-WyjAz.otf</t>
-  </si>
-  <si>
     <t>ZinfandelSpurRegular-qJr0.ttf</t>
   </si>
   <si>
@@ -348,9 +273,6 @@
     <t>fast99.ttf</t>
   </si>
   <si>
-    <t>zawijasy.otf</t>
-  </si>
-  <si>
     <t>GloriousChristmas-BLWWB.ttf</t>
   </si>
   <si>
@@ -373,6 +295,84 @@
   </si>
   <si>
     <t>Tempo</t>
+  </si>
+  <si>
+    <t>RockRadio-Wy4Vz.ttf</t>
+  </si>
+  <si>
+    <t>RockSlayers-BW6Lw.ttf</t>
+  </si>
+  <si>
+    <t>TigerChest-yw6Le.ttf</t>
+  </si>
+  <si>
+    <t>BeautySwingPersonalUse-DOEaD.ttf</t>
+  </si>
+  <si>
+    <t>MEllington.ttf</t>
+  </si>
+  <si>
+    <t>OPTINovelGothic-XBoldAgen.ttf</t>
+  </si>
+  <si>
+    <t>RumbleweedspurRegular-VwLy.ttf</t>
+  </si>
+  <si>
+    <t>UnchainedRoughPersonalUseRegular-WyjAz.ttf</t>
+  </si>
+  <si>
+    <t>BombDaGone-VG0RB.ttf</t>
+  </si>
+  <si>
+    <t>DonGraffiti-wrYx.ttf</t>
+  </si>
+  <si>
+    <t>GraffitiHipsterDemoVersionRegular-ZVBxJ.ttf</t>
+  </si>
+  <si>
+    <t>MarleyRegular-zM1a.ttf</t>
+  </si>
+  <si>
+    <t>zawijasy.ttf</t>
+  </si>
+  <si>
+    <t>CrushMetal-8MP7A.ttf</t>
+  </si>
+  <si>
+    <t>DeadeldermetalRegular-1Gx3v.ttf</t>
+  </si>
+  <si>
+    <t>70SdiscopersonaluseBold-w14z2.ttf</t>
+  </si>
+  <si>
+    <t>DiscoDeck-a4wa.ttf</t>
+  </si>
+  <si>
+    <t>DiscoDuck3DItalic-al1m.ttf</t>
+  </si>
+  <si>
+    <t>MoogieDisco-2OwAX.ttf</t>
+  </si>
+  <si>
+    <t>AutumnFlowers-9YVZK.ttf</t>
+  </si>
+  <si>
+    <t>ClassicSignatureDemo-axdDE.ttf</t>
+  </si>
+  <si>
+    <t>Classical-4pq9.ttf</t>
+  </si>
+  <si>
+    <t>ElegantDemo-OVJX6.ttf</t>
+  </si>
+  <si>
+    <t>ElegantStylish-JR3xj.ttf</t>
+  </si>
+  <si>
+    <t>Faldith-qZM95.ttf</t>
+  </si>
+  <si>
+    <t>RusillaSerif-2OZpl.ttf</t>
   </si>
 </sst>
 </file>
@@ -752,7 +752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC8A9F8-F6F7-C446-981F-A14B4FAC156C}">
   <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -771,10 +771,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -830,7 +830,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -838,7 +838,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -846,7 +846,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -854,7 +854,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -862,7 +862,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -870,7 +870,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -878,7 +878,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -886,7 +886,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -894,7 +894,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -902,7 +902,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -910,7 +910,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -918,7 +918,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -926,7 +926,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -934,7 +934,7 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -942,7 +942,7 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -950,7 +950,7 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -958,7 +958,7 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -966,7 +966,7 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -974,7 +974,7 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -982,7 +982,7 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -990,7 +990,7 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -998,7 +998,7 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1006,7 +1006,7 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1022,7 +1022,7 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1030,7 +1030,7 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1038,7 +1038,7 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1046,7 +1046,7 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1054,7 +1054,7 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1062,7 +1062,7 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -1070,7 +1070,7 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1078,7 +1078,7 @@
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1086,7 +1086,7 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -1094,7 +1094,7 @@
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -1102,7 +1102,7 @@
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -1110,7 +1110,7 @@
         <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -1118,7 +1118,7 @@
         <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -1126,7 +1126,7 @@
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -1134,7 +1134,7 @@
         <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1142,7 +1142,7 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1150,7 +1150,7 @@
         <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1158,7 +1158,7 @@
         <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1166,7 +1166,7 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1174,7 +1174,7 @@
         <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1182,7 +1182,7 @@
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -1190,7 +1190,7 @@
         <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -1198,7 +1198,7 @@
         <v>7</v>
       </c>
       <c r="B54" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1206,7 +1206,7 @@
         <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -1214,7 +1214,7 @@
         <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -1222,7 +1222,7 @@
         <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -1230,7 +1230,7 @@
         <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -1238,7 +1238,7 @@
         <v>7</v>
       </c>
       <c r="B59" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -1246,7 +1246,7 @@
         <v>7</v>
       </c>
       <c r="B60" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -1254,7 +1254,7 @@
         <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -1262,7 +1262,7 @@
         <v>8</v>
       </c>
       <c r="B62" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -1270,7 +1270,7 @@
         <v>8</v>
       </c>
       <c r="B63" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -1278,7 +1278,7 @@
         <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -1286,7 +1286,7 @@
         <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -1294,7 +1294,7 @@
         <v>8</v>
       </c>
       <c r="B66" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -1302,7 +1302,7 @@
         <v>8</v>
       </c>
       <c r="B67" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -1310,7 +1310,7 @@
         <v>8</v>
       </c>
       <c r="B68" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -1318,7 +1318,7 @@
         <v>8</v>
       </c>
       <c r="B69" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -1326,7 +1326,7 @@
         <v>8</v>
       </c>
       <c r="B70" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -1334,7 +1334,7 @@
         <v>9</v>
       </c>
       <c r="B71" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -1342,7 +1342,7 @@
         <v>9</v>
       </c>
       <c r="B72" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -1350,7 +1350,7 @@
         <v>9</v>
       </c>
       <c r="B73" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -1358,7 +1358,7 @@
         <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -1366,7 +1366,7 @@
         <v>9</v>
       </c>
       <c r="B75" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -1374,7 +1374,7 @@
         <v>9</v>
       </c>
       <c r="B76" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -1382,7 +1382,7 @@
         <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -1390,7 +1390,7 @@
         <v>9</v>
       </c>
       <c r="B78" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
@@ -1398,7 +1398,7 @@
         <v>9</v>
       </c>
       <c r="B79" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -1406,7 +1406,7 @@
         <v>9</v>
       </c>
       <c r="B80" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -1414,7 +1414,7 @@
         <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -1422,7 +1422,7 @@
         <v>10</v>
       </c>
       <c r="B82" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
@@ -1430,7 +1430,7 @@
         <v>10</v>
       </c>
       <c r="B83" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
@@ -1438,7 +1438,7 @@
         <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -1446,7 +1446,7 @@
         <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
@@ -1454,7 +1454,7 @@
         <v>10</v>
       </c>
       <c r="B86" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -1462,7 +1462,7 @@
         <v>10</v>
       </c>
       <c r="B87" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
@@ -1470,7 +1470,7 @@
         <v>10</v>
       </c>
       <c r="B88" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
@@ -1478,7 +1478,7 @@
         <v>10</v>
       </c>
       <c r="B89" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
@@ -1486,7 +1486,7 @@
         <v>10</v>
       </c>
       <c r="B90" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
@@ -1494,7 +1494,7 @@
         <v>11</v>
       </c>
       <c r="B91" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
@@ -1502,7 +1502,7 @@
         <v>11</v>
       </c>
       <c r="B92" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
@@ -1510,7 +1510,7 @@
         <v>11</v>
       </c>
       <c r="B93" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
@@ -1518,7 +1518,7 @@
         <v>11</v>
       </c>
       <c r="B94" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
@@ -1526,7 +1526,7 @@
         <v>11</v>
       </c>
       <c r="B95" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
@@ -1534,7 +1534,7 @@
         <v>11</v>
       </c>
       <c r="B96" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
@@ -1542,7 +1542,7 @@
         <v>11</v>
       </c>
       <c r="B97" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -1550,7 +1550,7 @@
         <v>11</v>
       </c>
       <c r="B98" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
@@ -1558,7 +1558,7 @@
         <v>11</v>
       </c>
       <c r="B99" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -1566,7 +1566,7 @@
         <v>11</v>
       </c>
       <c r="B100" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>